<commit_message>
RFS009, 010, 011 e 012 implementados e funcionais
</commit_message>
<xml_diff>
--- a/Documentação/Estimativa de tamanho de projeto - Plataforma de Crowdfunding.xlsx
+++ b/Documentação/Estimativa de tamanho de projeto - Plataforma de Crowdfunding.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CrowdFunding_Project\Documentação\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Pontos de Casos de Uso" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -481,7 +485,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -833,7 +837,7 @@
     <xf numFmtId="9" fontId="9" fillId="12" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="12" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -842,22 +846,53 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -895,9 +930,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -932,7 +967,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -967,7 +1002,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1144,7 +1179,7 @@
   <dimension ref="A1:M117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>